<commit_message>
Add some backdated FY basic metrics
</commit_message>
<xml_diff>
--- a/£SGE.xlsx
+++ b/£SGE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8428E47-851E-AE40-9DB2-B9FC615FD7A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA68B143-821E-46FB-B186-0A6961700E26}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33080" windowHeight="18480" activeTab="1" xr2:uid="{E05933DB-826C-48C0-AE9A-F8A61FB6D502}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="33075" windowHeight="18480" xr2:uid="{E05933DB-826C-48C0-AE9A-F8A61FB6D502}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -21,22 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="104">
   <si>
     <t>£SGE</t>
   </si>
@@ -345,18 +335,20 @@
   </si>
   <si>
     <t>H123</t>
+  </si>
+  <si>
+    <t>EV/S</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0.0\x"/>
-    <numFmt numFmtId="168" formatCode="0.00\x"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -651,24 +643,7 @@
     <xf numFmtId="166" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -693,13 +668,26 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -844,8 +832,8 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -860,8 +848,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9569450" y="9525"/>
-          <a:ext cx="0" cy="12030075"/>
+          <a:off x="6940550" y="9525"/>
+          <a:ext cx="0" cy="13439775"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -894,8 +882,8 @@
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -910,8 +898,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16725900" y="0"/>
-          <a:ext cx="0" cy="12360275"/>
+          <a:off x="14249400" y="0"/>
+          <a:ext cx="0" cy="13677900"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1236,65 +1224,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB50BB21-6927-4998-A7CD-B755108AED34}">
   <dimension ref="A2:X34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F2"/>
-      <c r="G2" s="50" t="s">
+      <c r="G2" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="B5" s="51" t="s">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B5" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="53"/>
-      <c r="H5" s="51" t="s">
+      <c r="C5" s="60"/>
+      <c r="D5" s="61"/>
+      <c r="H5" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="I5" s="52"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="52"/>
-      <c r="Q5" s="53"/>
-      <c r="T5" s="51" t="s">
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="60"/>
+      <c r="M5" s="60"/>
+      <c r="N5" s="60"/>
+      <c r="O5" s="60"/>
+      <c r="P5" s="60"/>
+      <c r="Q5" s="61"/>
+      <c r="T5" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="U5" s="52"/>
-      <c r="V5" s="52"/>
-      <c r="W5" s="52"/>
-      <c r="X5" s="53"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="U5" s="60"/>
+      <c r="V5" s="60"/>
+      <c r="W5" s="60"/>
+      <c r="X5" s="61"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="66">
+      <c r="C6" s="50">
         <v>8.0571999999999999</v>
       </c>
       <c r="D6" s="14"/>
@@ -1316,7 +1304,7 @@
       <c r="W6" s="7"/>
       <c r="X6" s="8"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
@@ -1342,7 +1330,7 @@
       <c r="W7" s="7"/>
       <c r="X7" s="8"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
@@ -1367,7 +1355,7 @@
       <c r="W8" s="7"/>
       <c r="X8" s="8"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
@@ -1394,7 +1382,7 @@
       <c r="W9" s="7"/>
       <c r="X9" s="8"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
@@ -1421,7 +1409,7 @@
       <c r="W10" s="7"/>
       <c r="X10" s="8"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
@@ -1448,7 +1436,7 @@
       <c r="W11" s="7"/>
       <c r="X11" s="8"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
@@ -1473,7 +1461,7 @@
       <c r="W12" s="7"/>
       <c r="X12" s="8"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="H13" s="12"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
@@ -1490,7 +1478,7 @@
       <c r="W13" s="10"/>
       <c r="X13" s="11"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="H14" s="12"/>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
@@ -1502,12 +1490,12 @@
       <c r="P14" s="7"/>
       <c r="Q14" s="8"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="B15" s="51" t="s">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B15" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="52"/>
-      <c r="D15" s="53"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="61"/>
       <c r="H15" s="12"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
@@ -1519,17 +1507,17 @@
       <c r="P15" s="7"/>
       <c r="Q15" s="8"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="60" t="s">
+      <c r="C16" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="61"/>
+      <c r="D16" s="56"/>
       <c r="E16" s="1" t="s">
         <v>25</v>
       </c>
@@ -1544,17 +1532,17 @@
       <c r="P16" s="7"/>
       <c r="Q16" s="8"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
         <v>26</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="60" t="s">
+      <c r="C17" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="61"/>
+      <c r="D17" s="56"/>
       <c r="H17" s="12"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
@@ -1566,14 +1554,14 @@
       <c r="P17" s="7"/>
       <c r="Q17" s="8"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B18" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="60" t="s">
+      <c r="C18" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="61"/>
+      <c r="D18" s="56"/>
       <c r="H18" s="12"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
@@ -1585,14 +1573,14 @@
       <c r="P18" s="7"/>
       <c r="Q18" s="8"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B19" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="62" t="s">
+      <c r="C19" s="57" t="s">
         <v>97</v>
       </c>
-      <c r="D19" s="63"/>
+      <c r="D19" s="58"/>
       <c r="H19" s="12"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
@@ -1604,7 +1592,7 @@
       <c r="P19" s="7"/>
       <c r="Q19" s="8"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H20" s="12"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
@@ -1616,7 +1604,7 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H21" s="12"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
@@ -1628,12 +1616,12 @@
       <c r="P21" s="7"/>
       <c r="Q21" s="8"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="B22" s="51" t="s">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B22" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="52"/>
-      <c r="D22" s="53"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="61"/>
       <c r="H22" s="12"/>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
@@ -1645,14 +1633,14 @@
       <c r="P22" s="7"/>
       <c r="Q22" s="8"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B23" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="60" t="s">
+      <c r="C23" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="61"/>
+      <c r="D23" s="56"/>
       <c r="H23" s="12"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
@@ -1664,14 +1652,14 @@
       <c r="P23" s="7"/>
       <c r="Q23" s="8"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B24" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="60">
+      <c r="C24" s="55">
         <v>1981</v>
       </c>
-      <c r="D24" s="61"/>
+      <c r="D24" s="56"/>
       <c r="H24" s="12"/>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
@@ -1683,10 +1671,10 @@
       <c r="P24" s="7"/>
       <c r="Q24" s="8"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B25" s="12"/>
-      <c r="C25" s="60"/>
-      <c r="D25" s="61"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="56"/>
       <c r="H25" s="12"/>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
@@ -1698,10 +1686,10 @@
       <c r="P25" s="7"/>
       <c r="Q25" s="8"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B26" s="12"/>
-      <c r="C26" s="60"/>
-      <c r="D26" s="61"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="56"/>
       <c r="H26" s="12"/>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
@@ -1713,7 +1701,7 @@
       <c r="P26" s="7"/>
       <c r="Q26" s="8"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B27" s="12" t="s">
         <v>17</v>
       </c>
@@ -1734,14 +1722,14 @@
       <c r="P27" s="7"/>
       <c r="Q27" s="8"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B28" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="64" t="s">
+      <c r="C28" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="65"/>
+      <c r="D28" s="63"/>
       <c r="H28" s="12"/>
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
@@ -1753,7 +1741,7 @@
       <c r="P28" s="7"/>
       <c r="Q28" s="8"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H29" s="12"/>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
@@ -1765,7 +1753,7 @@
       <c r="P29" s="7"/>
       <c r="Q29" s="8"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H30" s="12"/>
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
@@ -1777,12 +1765,12 @@
       <c r="P30" s="7"/>
       <c r="Q30" s="8"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="B31" s="51" t="s">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B31" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="52"/>
-      <c r="D31" s="53"/>
+      <c r="C31" s="60"/>
+      <c r="D31" s="61"/>
       <c r="H31" s="12"/>
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
@@ -1794,15 +1782,15 @@
       <c r="P31" s="7"/>
       <c r="Q31" s="8"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B32" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="54">
-        <f>C6/(('Financial Model'!I14+'Financial Model'!H14))</f>
-        <v>29.057331309550619</v>
-      </c>
-      <c r="D32" s="55"/>
+      <c r="C32" s="51">
+        <f>C6/'Financial Model'!V14</f>
+        <v>32.35568503937008</v>
+      </c>
+      <c r="D32" s="52"/>
       <c r="H32" s="12"/>
       <c r="I32" s="7"/>
       <c r="J32" s="7"/>
@@ -1814,15 +1802,15 @@
       <c r="P32" s="7"/>
       <c r="Q32" s="8"/>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B33" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="56">
-        <f>C8/SUM('Financial Model'!H4:I4)</f>
-        <v>4.4592208355941398</v>
-      </c>
-      <c r="D33" s="57"/>
+      <c r="C33" s="51">
+        <f>C8/'Financial Model'!V4</f>
+        <v>4.2210292758089363</v>
+      </c>
+      <c r="D33" s="52"/>
       <c r="H33" s="12"/>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
@@ -1834,15 +1822,15 @@
       <c r="P33" s="7"/>
       <c r="Q33" s="8"/>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B34" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="58">
-        <f>C6/'Financial Model'!I61</f>
-        <v>6.8459431893687706</v>
-      </c>
-      <c r="D34" s="59"/>
+      <c r="C34" s="53">
+        <f>C6/'Financial Model'!V61</f>
+        <v>5.9682962962962955</v>
+      </c>
+      <c r="D34" s="54"/>
       <c r="H34" s="13"/>
       <c r="I34" s="10"/>
       <c r="J34" s="10"/>
@@ -1856,6 +1844,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="G2:L2"/>
+    <mergeCell ref="H5:Q5"/>
+    <mergeCell ref="T5:X5"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B15:D15"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="C16:D16"/>
@@ -1868,13 +1863,6 @@
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C23:D23"/>
-    <mergeCell ref="G2:L2"/>
-    <mergeCell ref="H5:Q5"/>
-    <mergeCell ref="T5:X5"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B15:D15"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C28:D28" r:id="rId1" display="Link" xr:uid="{E398FABE-A8E2-41B0-BEEF-891546DA9EBE}"/>
@@ -1887,31 +1875,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFBB68F3-0B4D-4779-B224-181DBEE6F8C1}">
-  <dimension ref="B1:AE69"/>
+  <dimension ref="B1:AE74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomRight" activeCell="Z70" sqref="Z70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" style="1"/>
-    <col min="4" max="4" width="9.1640625" style="23"/>
-    <col min="5" max="5" width="9.1640625" style="1"/>
-    <col min="6" max="6" width="9.1640625" style="23"/>
-    <col min="7" max="7" width="9.1640625" style="1"/>
-    <col min="8" max="8" width="9.1640625" style="23"/>
-    <col min="9" max="9" width="9.1640625" style="1"/>
-    <col min="10" max="10" width="9.1640625" style="23"/>
-    <col min="11" max="16384" width="9.1640625" style="1"/>
+    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="9.140625" style="23"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="9.140625" style="23"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="9.140625" style="23"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="9.140625" style="23"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:31" s="21" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:31" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C1" s="21" t="s">
         <v>32</v>
       </c>
@@ -1982,7 +1970,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="2:31" s="26" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:31" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="25"/>
       <c r="C2" s="29">
         <v>43555</v>
@@ -2026,7 +2014,7 @@
         <v>44834</v>
       </c>
     </row>
-    <row r="3" spans="2:31" s="26" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:31" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="25"/>
       <c r="D3" s="46">
         <f>S3</f>
@@ -2056,7 +2044,7 @@
         <v>44881</v>
       </c>
     </row>
-    <row r="4" spans="2:31" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>39</v>
       </c>
@@ -2104,7 +2092,7 @@
         <v>1947</v>
       </c>
     </row>
-    <row r="5" spans="2:31" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>40</v>
       </c>
@@ -2152,7 +2140,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="2:31" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>41</v>
       </c>
@@ -2209,7 +2197,7 @@
         <v>1809</v>
       </c>
     </row>
-    <row r="7" spans="2:31" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>42</v>
       </c>
@@ -2257,7 +2245,7 @@
         <v>1442</v>
       </c>
     </row>
-    <row r="8" spans="2:31" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>43</v>
       </c>
@@ -2314,7 +2302,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="9" spans="2:31" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>44</v>
       </c>
@@ -2362,7 +2350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:31" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>45</v>
       </c>
@@ -2410,7 +2398,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="2:31" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>46</v>
       </c>
@@ -2467,7 +2455,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="12" spans="2:31" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>47</v>
       </c>
@@ -2515,7 +2503,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="2:31" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>48</v>
       </c>
@@ -2572,7 +2560,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="14" spans="2:31" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>49</v>
       </c>
@@ -2629,7 +2617,7 @@
         <v>0.24901960784313726</v>
       </c>
     </row>
-    <row r="15" spans="2:31" s="32" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:31" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B15" s="32" t="s">
         <v>4</v>
       </c>
@@ -2677,7 +2665,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>52</v>
       </c>
@@ -2734,7 +2722,7 @@
         <v>0.92912172573189522</v>
       </c>
     </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>53</v>
       </c>
@@ -2791,7 +2779,7 @@
         <v>0.18849512069851052</v>
       </c>
     </row>
-    <row r="19" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>54</v>
       </c>
@@ -2848,7 +2836,7 @@
         <v>0.13045711350796096</v>
       </c>
     </row>
-    <row r="20" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>100</v>
       </c>
@@ -2905,7 +2893,7 @@
         <v>0.24629080118694363</v>
       </c>
     </row>
-    <row r="22" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>50</v>
       </c>
@@ -2916,38 +2904,38 @@
         <v>92</v>
       </c>
       <c r="E22" s="35">
-        <f>E4/C4-1</f>
+        <f t="shared" ref="E22:J22" si="23">E4/C4-1</f>
         <v>1.8808777429467183E-2</v>
       </c>
       <c r="F22" s="45">
-        <f>F4/D4-1</f>
+        <f t="shared" si="23"/>
         <v>-5.2093973442288055E-2</v>
       </c>
       <c r="G22" s="35">
-        <f>G4/E4-1</f>
+        <f t="shared" si="23"/>
         <v>-3.8974358974358969E-2</v>
       </c>
       <c r="H22" s="45">
-        <f>H4/F4-1</f>
+        <f t="shared" si="23"/>
         <v>-2.0474137931034475E-2</v>
       </c>
       <c r="I22" s="35">
-        <f>I4/G4-1</f>
+        <f t="shared" si="23"/>
         <v>-3.2017075773745907E-3</v>
       </c>
       <c r="J22" s="45">
-        <f>J4/H4-1</f>
+        <f t="shared" si="23"/>
         <v>0.11441144114411439</v>
       </c>
       <c r="R22" s="19" t="s">
         <v>92</v>
       </c>
       <c r="S22" s="43">
-        <f t="shared" ref="S22:T22" si="23">S4/R4-1</f>
+        <f t="shared" ref="S22:T22" si="24">S4/R4-1</f>
         <v>4.8754062838569867E-2</v>
       </c>
       <c r="T22" s="43">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>-1.7045454545454586E-2</v>
       </c>
       <c r="U22" s="43">
@@ -2955,11 +2943,11 @@
         <v>-2.9952706253284278E-2</v>
       </c>
       <c r="V22" s="43">
-        <f t="shared" ref="V22" si="24">V4/U4-1</f>
+        <f t="shared" ref="V22" si="25">V4/U4-1</f>
         <v>5.4712892741061836E-2</v>
       </c>
     </row>
-    <row r="23" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>51</v>
       </c>
@@ -2967,31 +2955,31 @@
         <v>92</v>
       </c>
       <c r="D23" s="44">
-        <f t="shared" ref="D23:J23" si="25">D4/C4-1</f>
+        <f t="shared" ref="D23:J23" si="26">D4/C4-1</f>
         <v>2.2988505747126409E-2</v>
       </c>
       <c r="E23" s="31">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>-4.0858018386108474E-3</v>
       </c>
       <c r="F23" s="44">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>-4.8205128205128234E-2</v>
       </c>
       <c r="G23" s="31">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>9.6982758620689502E-3</v>
       </c>
       <c r="H23" s="44">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>-2.9882604055496254E-2</v>
       </c>
       <c r="I23" s="31">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>2.7502750275027577E-2</v>
       </c>
       <c r="J23" s="44">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>8.4582441113490336E-2</v>
       </c>
       <c r="R23" s="19" t="s">
@@ -3010,12 +2998,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B27" s="36" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>70</v>
       </c>
@@ -3072,7 +3060,7 @@
         <v>2710</v>
       </c>
     </row>
-    <row r="29" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>71</v>
       </c>
@@ -3118,7 +3106,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="30" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
         <v>72</v>
       </c>
@@ -3164,7 +3152,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
         <v>73</v>
       </c>
@@ -3191,7 +3179,7 @@
         <v>0</v>
       </c>
       <c r="J31" s="23">
-        <f t="shared" ref="J31:J38" si="26">-V31</f>
+        <f t="shared" ref="J31:J38" si="27">-V31</f>
         <v>0</v>
       </c>
       <c r="R31" s="37">
@@ -3210,7 +3198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>74</v>
       </c>
@@ -3224,7 +3212,7 @@
         <v>83</v>
       </c>
       <c r="F32" s="33">
-        <f t="shared" ref="F32:F38" si="27">T32</f>
+        <f t="shared" ref="F32:F38" si="28">T32</f>
         <v>86</v>
       </c>
       <c r="G32" s="32">
@@ -3237,7 +3225,7 @@
         <v>116</v>
       </c>
       <c r="J32" s="23">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>-128</v>
       </c>
       <c r="R32" s="32">
@@ -3256,7 +3244,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="33" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
         <v>75</v>
       </c>
@@ -3270,7 +3258,7 @@
         <v>26</v>
       </c>
       <c r="F33" s="33">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>35</v>
       </c>
       <c r="G33" s="32">
@@ -3283,7 +3271,7 @@
         <v>34</v>
       </c>
       <c r="J33" s="23">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>-19</v>
       </c>
       <c r="R33" s="32">
@@ -3302,40 +3290,40 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>76</v>
       </c>
       <c r="C34" s="32">
-        <f t="shared" ref="C34:J34" si="28">SUM(C28:C33)</f>
+        <f t="shared" ref="C34:J34" si="29">SUM(C28:C33)</f>
         <v>2471</v>
       </c>
       <c r="D34" s="33">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>2551</v>
       </c>
       <c r="E34" s="32">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>2585</v>
       </c>
       <c r="F34" s="33">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>2469</v>
       </c>
       <c r="G34" s="32">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>2353</v>
       </c>
       <c r="H34" s="33">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>2405</v>
       </c>
       <c r="I34" s="32">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>2672</v>
       </c>
       <c r="J34" s="33">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>2415</v>
       </c>
       <c r="R34" s="32">
@@ -3359,7 +3347,7 @@
         <v>3013</v>
       </c>
     </row>
-    <row r="35" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>74</v>
       </c>
@@ -3373,7 +3361,7 @@
         <v>329</v>
       </c>
       <c r="F35" s="33">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>302</v>
       </c>
       <c r="G35" s="32">
@@ -3386,7 +3374,7 @@
         <v>329</v>
       </c>
       <c r="J35" s="23">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>-335</v>
       </c>
       <c r="R35" s="32">
@@ -3405,7 +3393,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="36" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>77</v>
       </c>
@@ -3419,7 +3407,7 @@
         <v>15</v>
       </c>
       <c r="F36" s="33">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>5</v>
       </c>
       <c r="G36" s="32">
@@ -3432,7 +3420,7 @@
         <v>28</v>
       </c>
       <c r="J36" s="23">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>-39</v>
       </c>
       <c r="R36" s="32">
@@ -3451,7 +3439,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
         <v>6</v>
       </c>
@@ -3502,7 +3490,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="38" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="38" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
         <v>78</v>
       </c>
@@ -3516,7 +3504,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="33">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>108</v>
       </c>
       <c r="G38" s="32">
@@ -3529,7 +3517,7 @@
         <v>2</v>
       </c>
       <c r="J38" s="23">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="R38" s="32">
@@ -3548,40 +3536,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="39" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>79</v>
       </c>
       <c r="C39" s="32">
-        <f t="shared" ref="C39:J39" si="29">C34+SUM(C35:C38)</f>
+        <f t="shared" ref="C39:J39" si="30">C34+SUM(C35:C38)</f>
         <v>3228</v>
       </c>
       <c r="D39" s="33">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>3352</v>
       </c>
       <c r="E39" s="32">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>3841</v>
       </c>
       <c r="F39" s="33">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>3715</v>
       </c>
       <c r="G39" s="32">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>3444</v>
       </c>
       <c r="H39" s="33">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>3329</v>
       </c>
       <c r="I39" s="32">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>3546</v>
       </c>
       <c r="J39" s="33">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>2530</v>
       </c>
       <c r="R39" s="32">
@@ -3605,7 +3593,7 @@
         <v>3876</v>
       </c>
     </row>
-    <row r="40" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="40" spans="2:22" x14ac:dyDescent="0.2">
       <c r="G40" s="32"/>
       <c r="H40" s="33"/>
       <c r="R40" s="32"/>
@@ -3613,7 +3601,7 @@
       <c r="T40" s="32"/>
       <c r="U40" s="32"/>
     </row>
-    <row r="41" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="41" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
         <v>80</v>
       </c>
@@ -3627,7 +3615,7 @@
         <v>242</v>
       </c>
       <c r="F41" s="33">
-        <f t="shared" ref="F41:F46" si="30">T41</f>
+        <f t="shared" ref="F41:F46" si="31">T41</f>
         <v>297</v>
       </c>
       <c r="G41" s="32">
@@ -3640,7 +3628,7 @@
         <v>311</v>
       </c>
       <c r="J41" s="23">
-        <f>V41</f>
+        <f t="shared" ref="J41:J46" si="32">V41</f>
         <v>368</v>
       </c>
       <c r="R41" s="32">
@@ -3659,7 +3647,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="42" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="42" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
         <v>77</v>
       </c>
@@ -3673,7 +3661,7 @@
         <v>46</v>
       </c>
       <c r="F42" s="33">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>13</v>
       </c>
       <c r="G42" s="32">
@@ -3686,7 +3674,7 @@
         <v>23</v>
       </c>
       <c r="J42" s="23">
-        <f>V42</f>
+        <f t="shared" si="32"/>
         <v>13</v>
       </c>
       <c r="R42" s="32">
@@ -3705,7 +3693,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B43" s="2" t="s">
         <v>81</v>
       </c>
@@ -3732,7 +3720,7 @@
         <v>42</v>
       </c>
       <c r="J43" s="30">
-        <f>V43</f>
+        <f t="shared" si="32"/>
         <v>178</v>
       </c>
       <c r="M43" s="1"/>
@@ -3756,7 +3744,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="44" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="44" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
         <v>82</v>
       </c>
@@ -3770,7 +3758,7 @@
         <v>9</v>
       </c>
       <c r="F44" s="33">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>19</v>
       </c>
       <c r="G44" s="32">
@@ -3783,7 +3771,7 @@
         <v>44</v>
       </c>
       <c r="J44" s="23">
-        <f>V44</f>
+        <f t="shared" si="32"/>
         <v>33</v>
       </c>
       <c r="R44" s="32">
@@ -3802,7 +3790,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="45" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
         <v>83</v>
       </c>
@@ -3816,7 +3804,7 @@
         <v>691</v>
       </c>
       <c r="F45" s="33">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>593</v>
       </c>
       <c r="G45" s="32">
@@ -3829,7 +3817,7 @@
         <v>705</v>
       </c>
       <c r="J45" s="23">
-        <f>V45</f>
+        <f t="shared" si="32"/>
         <v>734</v>
       </c>
       <c r="R45" s="32">
@@ -3848,7 +3836,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="46" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="46" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
         <v>86</v>
       </c>
@@ -3862,7 +3850,7 @@
         <v>0</v>
       </c>
       <c r="F46" s="33">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>73</v>
       </c>
       <c r="G46" s="32">
@@ -3875,7 +3863,7 @@
         <v>0</v>
       </c>
       <c r="J46" s="23">
-        <f>V46</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R46" s="32">
@@ -3894,40 +3882,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="47" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C47" s="32">
-        <f t="shared" ref="C47:J47" si="31">SUM(C41:C46)</f>
+        <f t="shared" ref="C47:J47" si="33">SUM(C41:C46)</f>
         <v>1003</v>
       </c>
       <c r="D47" s="33">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>1126</v>
       </c>
       <c r="E47" s="32">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>1137</v>
       </c>
       <c r="F47" s="33">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>1015</v>
       </c>
       <c r="G47" s="32">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>1322</v>
       </c>
       <c r="H47" s="33">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>1380</v>
       </c>
       <c r="I47" s="32">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>1125</v>
       </c>
       <c r="J47" s="33">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>1326</v>
       </c>
       <c r="R47" s="32">
@@ -3951,7 +3939,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="48" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
         <v>81</v>
       </c>
@@ -3978,7 +3966,7 @@
         <v>1123</v>
       </c>
       <c r="J48" s="30">
-        <f>V48</f>
+        <f t="shared" ref="J48:J54" si="34">V48</f>
         <v>1044</v>
       </c>
       <c r="M48" s="1"/>
@@ -4002,7 +3990,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="49" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="49" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B49" s="1" t="s">
         <v>85</v>
       </c>
@@ -4016,7 +4004,7 @@
         <v>26</v>
       </c>
       <c r="F49" s="33">
-        <f t="shared" ref="F49:F53" si="32">T49</f>
+        <f t="shared" ref="F49:F53" si="35">T49</f>
         <v>23</v>
       </c>
       <c r="G49" s="32">
@@ -4029,7 +4017,7 @@
         <v>23</v>
       </c>
       <c r="J49" s="23">
-        <f>V49</f>
+        <f t="shared" si="34"/>
         <v>19</v>
       </c>
       <c r="R49" s="32">
@@ -4048,7 +4036,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="50" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
         <v>75</v>
       </c>
@@ -4062,7 +4050,7 @@
         <v>27</v>
       </c>
       <c r="F50" s="33">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>14</v>
       </c>
       <c r="G50" s="32">
@@ -4075,7 +4063,7 @@
         <v>24</v>
       </c>
       <c r="J50" s="23">
-        <f>V50</f>
+        <f t="shared" si="34"/>
         <v>16</v>
       </c>
       <c r="R50" s="32">
@@ -4094,7 +4082,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="51" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B51" s="1" t="s">
         <v>82</v>
       </c>
@@ -4108,7 +4096,7 @@
         <v>13</v>
       </c>
       <c r="F51" s="33">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>31</v>
       </c>
       <c r="G51" s="32">
@@ -4121,7 +4109,7 @@
         <v>36</v>
       </c>
       <c r="J51" s="23">
-        <f>V51</f>
+        <f t="shared" si="34"/>
         <v>20</v>
       </c>
       <c r="R51" s="32">
@@ -4140,7 +4128,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="52" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B52" s="1" t="s">
         <v>80</v>
       </c>
@@ -4154,7 +4142,7 @@
         <v>6</v>
       </c>
       <c r="F52" s="33">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>3</v>
       </c>
       <c r="G52" s="32">
@@ -4167,7 +4155,7 @@
         <v>2</v>
       </c>
       <c r="J52" s="23">
-        <f>V52</f>
+        <f t="shared" si="34"/>
         <v>6</v>
       </c>
       <c r="R52" s="32">
@@ -4186,7 +4174,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="53" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B53" s="1" t="s">
         <v>83</v>
       </c>
@@ -4200,7 +4188,7 @@
         <v>7</v>
       </c>
       <c r="F53" s="33">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>7</v>
       </c>
       <c r="G53" s="32">
@@ -4213,7 +4201,7 @@
         <v>9</v>
       </c>
       <c r="J53" s="23">
-        <f>V53</f>
+        <f t="shared" si="34"/>
         <v>8</v>
       </c>
       <c r="R53" s="32">
@@ -4232,7 +4220,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="54" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B54" s="1" t="s">
         <v>101</v>
       </c>
@@ -4258,7 +4246,7 @@
         <v>0</v>
       </c>
       <c r="J54" s="23">
-        <f>V54</f>
+        <f t="shared" si="34"/>
         <v>60</v>
       </c>
       <c r="R54" s="32">
@@ -4277,40 +4265,40 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="55" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B55" s="1" t="s">
         <v>84</v>
       </c>
       <c r="C55" s="32">
-        <f>C47+SUM(C48:C54)</f>
+        <f t="shared" ref="C55:J55" si="36">C47+SUM(C48:C54)</f>
         <v>1845</v>
       </c>
       <c r="D55" s="33">
-        <f>D47+SUM(D48:D54)</f>
+        <f t="shared" si="36"/>
         <v>1848</v>
       </c>
       <c r="E55" s="32">
-        <f>E47+SUM(E48:E54)</f>
+        <f t="shared" si="36"/>
         <v>2217</v>
       </c>
       <c r="F55" s="33">
-        <f>F47+SUM(F48:F54)</f>
+        <f t="shared" si="36"/>
         <v>2063</v>
       </c>
       <c r="G55" s="32">
-        <f>G47+SUM(G48:G54)</f>
+        <f t="shared" si="36"/>
         <v>2140</v>
       </c>
       <c r="H55" s="33">
-        <f>H47+SUM(H48:H54)</f>
+        <f t="shared" si="36"/>
         <v>2218</v>
       </c>
       <c r="I55" s="32">
-        <f>I47+SUM(I48:I54)</f>
+        <f t="shared" si="36"/>
         <v>2342</v>
       </c>
       <c r="J55" s="33">
-        <f>J47+SUM(J48:J54)</f>
+        <f t="shared" si="36"/>
         <v>2499</v>
       </c>
       <c r="R55" s="32">
@@ -4334,7 +4322,7 @@
         <v>2499</v>
       </c>
     </row>
-    <row r="56" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="56" spans="2:22" x14ac:dyDescent="0.2">
       <c r="G56" s="32"/>
       <c r="H56" s="33"/>
       <c r="R56" s="32"/>
@@ -4342,7 +4330,7 @@
       <c r="T56" s="32"/>
       <c r="U56" s="32"/>
     </row>
-    <row r="57" spans="2:22" s="32" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="2:22" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B57" s="32" t="s">
         <v>88</v>
       </c>
@@ -4388,40 +4376,40 @@
         <v>1397</v>
       </c>
     </row>
-    <row r="58" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="58" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B58" s="1" t="s">
         <v>89</v>
       </c>
       <c r="C58" s="32">
-        <f t="shared" ref="C58:J58" si="33">C57+C55</f>
+        <f t="shared" ref="C58:J58" si="37">C57+C55</f>
         <v>3228</v>
       </c>
       <c r="D58" s="33">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>3352</v>
       </c>
       <c r="E58" s="32">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>3841</v>
       </c>
       <c r="F58" s="33">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>3715</v>
       </c>
       <c r="G58" s="32">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>3444</v>
       </c>
       <c r="H58" s="33">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>3329</v>
       </c>
       <c r="I58" s="32">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>3546</v>
       </c>
       <c r="J58" s="33">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>3896</v>
       </c>
       <c r="R58" s="32">
@@ -4445,44 +4433,44 @@
         <v>3896</v>
       </c>
     </row>
-    <row r="59" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="59" spans="2:22" x14ac:dyDescent="0.2">
       <c r="G59" s="32"/>
       <c r="H59" s="33"/>
     </row>
-    <row r="60" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="60" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B60" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C60" s="32">
-        <f t="shared" ref="C60:I60" si="34">C39-C55</f>
+        <f t="shared" ref="C60:I60" si="38">C39-C55</f>
         <v>1383</v>
       </c>
       <c r="D60" s="33">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>1504</v>
       </c>
       <c r="E60" s="32">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>1624</v>
       </c>
       <c r="F60" s="33">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>1652</v>
       </c>
       <c r="G60" s="32">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>1304</v>
       </c>
       <c r="H60" s="33">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>1111</v>
       </c>
       <c r="I60" s="32">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>1204</v>
       </c>
       <c r="J60" s="33">
-        <f t="shared" ref="J60" si="35">J39-J55</f>
+        <f t="shared" ref="J60" si="39">J39-J55</f>
         <v>31</v>
       </c>
       <c r="R60" s="32">
@@ -4502,44 +4490,44 @@
         <v>1111</v>
       </c>
       <c r="V60" s="32">
-        <f t="shared" ref="V60" si="36">V39-V55</f>
+        <f t="shared" ref="V60" si="40">V39-V55</f>
         <v>1377</v>
       </c>
     </row>
-    <row r="61" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="61" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B61" s="1" t="s">
         <v>91</v>
       </c>
       <c r="C61" s="1">
-        <f t="shared" ref="C61:I61" si="37">C60/C15</f>
+        <f t="shared" ref="C61:I61" si="41">C60/C15</f>
         <v>1.2734806629834254</v>
       </c>
       <c r="D61" s="23">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>1.3848987108655617</v>
       </c>
       <c r="E61" s="1">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>1.489908256880734</v>
       </c>
       <c r="F61" s="23">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>1.5142071494042164</v>
       </c>
       <c r="G61" s="1">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>1.1919561243144423</v>
       </c>
       <c r="H61" s="23">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>1.0287037037037037</v>
       </c>
       <c r="I61" s="1">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>1.1769305962854351</v>
       </c>
       <c r="J61" s="23">
-        <f t="shared" ref="J61" si="38">J60/J15</f>
+        <f t="shared" ref="J61" si="42">J60/J15</f>
         <v>3.0392156862745098E-2</v>
       </c>
       <c r="R61" s="1">
@@ -4559,47 +4547,47 @@
         <v>1.0287037037037037</v>
       </c>
       <c r="V61" s="1">
-        <f t="shared" ref="V61" si="39">V60/V15</f>
+        <f t="shared" ref="V61" si="43">V60/V15</f>
         <v>1.35</v>
       </c>
     </row>
-    <row r="62" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="62" spans="2:22" x14ac:dyDescent="0.2">
       <c r="G62" s="32"/>
     </row>
-    <row r="63" spans="2:22" s="40" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="2:22" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B63" s="40" t="s">
         <v>6</v>
       </c>
       <c r="C63" s="41">
-        <f t="shared" ref="C63:I63" si="40">C37+C30+C31</f>
+        <f t="shared" ref="C63:I63" si="44">C37+C30+C31</f>
         <v>354</v>
       </c>
       <c r="D63" s="42">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>375</v>
       </c>
       <c r="E63" s="41">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>915</v>
       </c>
       <c r="F63" s="42">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>832</v>
       </c>
       <c r="G63" s="41">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>713</v>
       </c>
       <c r="H63" s="42">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>574</v>
       </c>
       <c r="I63" s="41">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>519</v>
       </c>
       <c r="J63" s="42">
-        <f t="shared" ref="J63" si="41">J37+J30+J31</f>
+        <f t="shared" ref="J63" si="45">J37+J30+J31</f>
         <v>493</v>
       </c>
       <c r="R63" s="41">
@@ -4619,44 +4607,44 @@
         <v>574</v>
       </c>
       <c r="V63" s="41">
-        <f t="shared" ref="V63" si="42">V37+V30+V31</f>
+        <f t="shared" ref="V63" si="46">V37+V30+V31</f>
         <v>493</v>
       </c>
     </row>
-    <row r="64" spans="2:22" s="40" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="2:22" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B64" s="40" t="s">
         <v>7</v>
       </c>
       <c r="C64" s="41">
-        <f t="shared" ref="C64:I64" si="43">C43+C48</f>
+        <f t="shared" ref="C64:I64" si="47">C43+C48</f>
         <v>773</v>
       </c>
       <c r="D64" s="42">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>765</v>
       </c>
       <c r="E64" s="41">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>1150</v>
       </c>
       <c r="F64" s="42">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>990</v>
       </c>
       <c r="G64" s="41">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>807</v>
       </c>
       <c r="H64" s="42">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>814</v>
       </c>
       <c r="I64" s="41">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>1165</v>
       </c>
       <c r="J64" s="42">
-        <f t="shared" ref="J64" si="44">J43+J48</f>
+        <f t="shared" ref="J64" si="48">J43+J48</f>
         <v>1222</v>
       </c>
       <c r="R64" s="41">
@@ -4676,44 +4664,44 @@
         <v>814</v>
       </c>
       <c r="V64" s="41">
-        <f t="shared" ref="V64" si="45">V43+V48</f>
+        <f t="shared" ref="V64" si="49">V43+V48</f>
         <v>1222</v>
       </c>
     </row>
-    <row r="65" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="65" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B65" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C65" s="32">
-        <f t="shared" ref="C65:I65" si="46">C63-C64</f>
+        <f t="shared" ref="C65:I65" si="50">C63-C64</f>
         <v>-419</v>
       </c>
       <c r="D65" s="33">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>-390</v>
       </c>
       <c r="E65" s="32">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>-235</v>
       </c>
       <c r="F65" s="33">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>-158</v>
       </c>
       <c r="G65" s="32">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>-94</v>
       </c>
       <c r="H65" s="33">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>-240</v>
       </c>
       <c r="I65" s="32">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>-646</v>
       </c>
       <c r="J65" s="33">
-        <f t="shared" ref="J65" si="47">J63-J64</f>
+        <f t="shared" ref="J65" si="51">J63-J64</f>
         <v>-729</v>
       </c>
       <c r="R65" s="32">
@@ -4733,26 +4721,181 @@
         <v>-240</v>
       </c>
       <c r="V65" s="32">
-        <f t="shared" ref="V65" si="48">V63-V64</f>
+        <f t="shared" ref="V65" si="52">V63-V64</f>
         <v>-729</v>
       </c>
     </row>
-    <row r="66" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="66" spans="2:22" x14ac:dyDescent="0.2">
       <c r="G66" s="32"/>
     </row>
-    <row r="67" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="67" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B67" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="68" spans="2:22" x14ac:dyDescent="0.15">
+      <c r="R67" s="1">
+        <v>5.3022</v>
+      </c>
+      <c r="S67" s="1">
+        <v>6.9139999999999997</v>
+      </c>
+      <c r="T67" s="1">
+        <v>7.2080000000000002</v>
+      </c>
+      <c r="U67" s="1">
+        <v>7.0960000000000001</v>
+      </c>
+      <c r="V67" s="1">
+        <v>6.9720000000000004</v>
+      </c>
+    </row>
+    <row r="68" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B68" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="69" spans="2:22" x14ac:dyDescent="0.15">
+      <c r="R68" s="65">
+        <f t="shared" ref="R68:U68" si="53">R67*R15</f>
+        <v>5742.2826000000005</v>
+      </c>
+      <c r="S68" s="65">
+        <f t="shared" si="53"/>
+        <v>7508.6039999999994</v>
+      </c>
+      <c r="T68" s="65">
+        <f t="shared" si="53"/>
+        <v>7863.9279999999999</v>
+      </c>
+      <c r="U68" s="65">
+        <f t="shared" si="53"/>
+        <v>7663.68</v>
+      </c>
+      <c r="V68" s="65">
+        <f>V67*V15</f>
+        <v>7111.4400000000005</v>
+      </c>
+    </row>
+    <row r="69" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B69" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="R69" s="32">
+        <f t="shared" ref="R69:U69" si="54">R68-R65</f>
+        <v>6390.2826000000005</v>
+      </c>
+      <c r="S69" s="32">
+        <f t="shared" si="54"/>
+        <v>7898.6039999999994</v>
+      </c>
+      <c r="T69" s="32">
+        <f t="shared" si="54"/>
+        <v>8021.9279999999999</v>
+      </c>
+      <c r="U69" s="32">
+        <f t="shared" si="54"/>
+        <v>7903.68</v>
+      </c>
+      <c r="V69" s="32">
+        <f>V68-V65</f>
+        <v>7840.4400000000005</v>
+      </c>
+    </row>
+    <row r="71" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B71" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R71" s="66">
+        <f t="shared" ref="R71:V71" si="55">R67/R61</f>
+        <v>4.3834218320610692</v>
+      </c>
+      <c r="S71" s="66">
+        <f t="shared" si="55"/>
+        <v>4.9924228723404251</v>
+      </c>
+      <c r="T71" s="66">
+        <f t="shared" si="55"/>
+        <v>4.760246973365617</v>
+      </c>
+      <c r="U71" s="66">
+        <f t="shared" si="55"/>
+        <v>6.8980018001800181</v>
+      </c>
+      <c r="V71" s="66">
+        <f>V67/V61</f>
+        <v>5.1644444444444444</v>
+      </c>
+    </row>
+    <row r="72" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B72" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R72" s="66">
+        <f t="shared" ref="R72:V72" si="56">R68/R4</f>
+        <v>3.1106622968580719</v>
+      </c>
+      <c r="S72" s="66">
+        <f t="shared" si="56"/>
+        <v>3.878411157024793</v>
+      </c>
+      <c r="T72" s="66">
+        <f t="shared" si="56"/>
+        <v>4.1323846558066206</v>
+      </c>
+      <c r="U72" s="66">
+        <f t="shared" si="56"/>
+        <v>4.1515059588299028</v>
+      </c>
+      <c r="V72" s="66">
+        <f>V68/V4</f>
+        <v>3.6525115562403703</v>
+      </c>
+    </row>
+    <row r="73" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B73" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="R73" s="66">
+        <f t="shared" ref="R73:V73" si="57">R69/R4</f>
+        <v>3.4616915492957747</v>
+      </c>
+      <c r="S73" s="66">
+        <f t="shared" si="57"/>
+        <v>4.0798574380165284</v>
+      </c>
+      <c r="T73" s="66">
+        <f t="shared" si="57"/>
+        <v>4.2154114555964268</v>
+      </c>
+      <c r="U73" s="66">
+        <f t="shared" si="57"/>
+        <v>4.2815167930660891</v>
+      </c>
+      <c r="V73" s="66">
+        <f>V69/V4</f>
+        <v>4.0269337442218802</v>
+      </c>
+    </row>
+    <row r="74" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B74" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R74" s="66">
+        <f t="shared" ref="R74:V74" si="58">R67/R14</f>
+        <v>19.465364745762713</v>
+      </c>
+      <c r="S74" s="66">
+        <f t="shared" si="58"/>
+        <v>28.227834586466162</v>
+      </c>
+      <c r="T74" s="66">
+        <f t="shared" si="58"/>
+        <v>25.367509677419356</v>
+      </c>
+      <c r="U74" s="66">
+        <f t="shared" si="58"/>
+        <v>26.890105263157896</v>
+      </c>
+      <c r="V74" s="66">
+        <f>V67/V14</f>
+        <v>27.997795275590551</v>
       </c>
     </row>
   </sheetData>
@@ -4764,9 +4907,10 @@
     <hyperlink ref="V1" r:id="rId5" xr:uid="{868025EF-C9E4-3A47-BE7A-AE4B223C1AF9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId6"/>
   <ignoredErrors>
     <ignoredError sqref="H6:H8 H11 F6:F8 F11 F13 D6:D8 D11 J6:J11 F34:F53 J29:J39 J47" formula="1"/>
   </ignoredErrors>
-  <drawing r:id="rId6"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>